<commit_message>
Validacoes no front despesa e modal receitas
</commit_message>
<xml_diff>
--- a/public/migracao/grupodespesas.xlsx
+++ b/public/migracao/grupodespesas.xlsx
@@ -435,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A207"/>
+  <dimension ref="A1:A208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -1895,6 +1895,13 @@
         </is>
       </c>
     </row>
+    <row outlineLevel="0" r="208">
+      <c r="A208" s="4" t="inlineStr">
+        <is>
+          <t>EMPRESTIMO/EMPRESA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>